<commit_message>
bell and whisttles wn the pilot scri[
</commit_message>
<xml_diff>
--- a/Stimuli.xlsx
+++ b/Stimuli.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -42,319 +42,319 @@
     <t>Animal</t>
   </si>
   <si>
-    <t>'axe'</t>
-  </si>
-  <si>
-    <t>'ball'</t>
-  </si>
-  <si>
-    <t>'baseball'</t>
-  </si>
-  <si>
-    <t>'camera'</t>
-  </si>
-  <si>
-    <t>'cash'</t>
-  </si>
-  <si>
-    <t>'cellphone'</t>
-  </si>
-  <si>
-    <t>'comb'</t>
-  </si>
-  <si>
-    <t>'corkscrew'</t>
-  </si>
-  <si>
-    <t>'dime'</t>
-  </si>
-  <si>
-    <t>'faucet'</t>
-  </si>
-  <si>
-    <t>'football'</t>
-  </si>
-  <si>
-    <t>'glass'</t>
-  </si>
-  <si>
-    <t>'hairbrush'</t>
-  </si>
-  <si>
-    <t>'hoe'</t>
-  </si>
-  <si>
-    <t>'key'</t>
-  </si>
-  <si>
-    <t>'keyboard'</t>
-  </si>
-  <si>
-    <t>'megaphone'</t>
-  </si>
-  <si>
-    <t>'pan'</t>
-  </si>
-  <si>
-    <t>'pen'</t>
-  </si>
-  <si>
-    <t>'pencil'</t>
-  </si>
-  <si>
-    <t>'rake'</t>
-  </si>
-  <si>
-    <t>'sandpaper'</t>
-  </si>
-  <si>
-    <t>'scissors'</t>
-  </si>
-  <si>
-    <t>'spatula'</t>
-  </si>
-  <si>
-    <t>'stapler'</t>
-  </si>
-  <si>
-    <t>'toaster'</t>
-  </si>
-  <si>
-    <t>'umbrella'</t>
-  </si>
-  <si>
-    <t>'beer'</t>
-  </si>
-  <si>
-    <t>'bread'</t>
-  </si>
-  <si>
-    <t>'cheese'</t>
-  </si>
-  <si>
-    <t>'chocolate'</t>
-  </si>
-  <si>
-    <t>'coffee'</t>
-  </si>
-  <si>
-    <t>'gum'</t>
-  </si>
-  <si>
-    <t>'ham'</t>
-  </si>
-  <si>
-    <t>'honey'</t>
-  </si>
-  <si>
-    <t>'jam'</t>
-  </si>
-  <si>
-    <t>'ketchup'</t>
-  </si>
-  <si>
-    <t>'lemonade'</t>
-  </si>
-  <si>
-    <t>'medicine'</t>
-  </si>
-  <si>
-    <t>'mustard'</t>
-  </si>
-  <si>
-    <t>'pie'</t>
-  </si>
-  <si>
-    <t>'rum'</t>
-  </si>
-  <si>
-    <t>'spaghetti'</t>
-  </si>
-  <si>
-    <t>'tea'</t>
-  </si>
-  <si>
-    <t>'tobacco'</t>
-  </si>
-  <si>
-    <t>'apricot'</t>
-  </si>
-  <si>
-    <t>'asparagus'</t>
-  </si>
-  <si>
-    <t>'banana'</t>
-  </si>
-  <si>
-    <t>'blueberry'</t>
-  </si>
-  <si>
-    <t>'broccoli'</t>
-  </si>
-  <si>
-    <t>'cabbage'</t>
-  </si>
-  <si>
-    <t>'carrot'</t>
-  </si>
-  <si>
-    <t>'cherry'</t>
-  </si>
-  <si>
-    <t>'chestnut'</t>
-  </si>
-  <si>
-    <t>'corn'</t>
-  </si>
-  <si>
-    <t>'cranberry'</t>
-  </si>
-  <si>
-    <t>'cucumber'</t>
-  </si>
-  <si>
-    <t>'dandelion'</t>
-  </si>
-  <si>
-    <t>'eggplant'</t>
-  </si>
-  <si>
-    <t>'elm'</t>
-  </si>
-  <si>
-    <t>'flower'</t>
-  </si>
-  <si>
-    <t>'ivy'</t>
-  </si>
-  <si>
-    <t>'mushroom'</t>
-  </si>
-  <si>
-    <t>'oak'</t>
-  </si>
-  <si>
-    <t>'pea'</t>
-  </si>
-  <si>
-    <t>'pineapple'</t>
-  </si>
-  <si>
-    <t>'plum'</t>
-  </si>
-  <si>
-    <t>'pumpkin'</t>
-  </si>
-  <si>
-    <t>'radish'</t>
-  </si>
-  <si>
-    <t>'raspberry'</t>
-  </si>
-  <si>
-    <t>'rose'</t>
-  </si>
-  <si>
-    <t>'tangerine'</t>
-  </si>
-  <si>
-    <t>'tomato'</t>
-  </si>
-  <si>
-    <t>'tree'</t>
-  </si>
-  <si>
-    <t>'tulip'</t>
-  </si>
-  <si>
-    <t>'alligator'</t>
-  </si>
-  <si>
-    <t>'ant'</t>
-  </si>
-  <si>
-    <t>'bee'</t>
-  </si>
-  <si>
-    <t>'bird'</t>
-  </si>
-  <si>
-    <t>'butterfly'</t>
-  </si>
-  <si>
-    <t>'camel'</t>
-  </si>
-  <si>
-    <t>'cheetah'</t>
-  </si>
-  <si>
-    <t>'chicken'</t>
-  </si>
-  <si>
-    <t>'chipmunk'</t>
-  </si>
-  <si>
-    <t>'crow'</t>
-  </si>
-  <si>
-    <t>'dog'</t>
-  </si>
-  <si>
-    <t>'dolphin'</t>
-  </si>
-  <si>
-    <t>'duck'</t>
-  </si>
-  <si>
-    <t>'elephant'</t>
-  </si>
-  <si>
-    <t>'fish'</t>
-  </si>
-  <si>
-    <t>'goldfish'</t>
-  </si>
-  <si>
-    <t>'hamster'</t>
-  </si>
-  <si>
-    <t>'hawk'</t>
-  </si>
-  <si>
-    <t>'horse'</t>
-  </si>
-  <si>
-    <t>'monkey'</t>
-  </si>
-  <si>
-    <t>'moose'</t>
-  </si>
-  <si>
-    <t>'mosquito'</t>
-  </si>
-  <si>
-    <t>'mouse'</t>
-  </si>
-  <si>
-    <t>'penguin'</t>
-  </si>
-  <si>
-    <t>'pig'</t>
-  </si>
-  <si>
-    <t>'salmon'</t>
-  </si>
-  <si>
-    <t>'snake'</t>
-  </si>
-  <si>
-    <t>'tiger'</t>
-  </si>
-  <si>
-    <t>'turtle'</t>
-  </si>
-  <si>
-    <t>'whale'</t>
+    <t>axe</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>apricot</t>
+  </si>
+  <si>
+    <t>alligator</t>
+  </si>
+  <si>
+    <t>ball</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>asparagus</t>
+  </si>
+  <si>
+    <t>ant</t>
+  </si>
+  <si>
+    <t>baseball</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>bee</t>
+  </si>
+  <si>
+    <t>camera</t>
+  </si>
+  <si>
+    <t>chocolate</t>
+  </si>
+  <si>
+    <t>blueberry</t>
+  </si>
+  <si>
+    <t>bird</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>broccoli</t>
+  </si>
+  <si>
+    <t>butterfly</t>
+  </si>
+  <si>
+    <t>cellphone</t>
+  </si>
+  <si>
+    <t>gum</t>
+  </si>
+  <si>
+    <t>cabbage</t>
+  </si>
+  <si>
+    <t>camel</t>
+  </si>
+  <si>
+    <t>comb</t>
+  </si>
+  <si>
+    <t>ham</t>
+  </si>
+  <si>
+    <t>carrot</t>
+  </si>
+  <si>
+    <t>cheetah</t>
+  </si>
+  <si>
+    <t>corkscrew</t>
+  </si>
+  <si>
+    <t>honey</t>
+  </si>
+  <si>
+    <t>cherry</t>
+  </si>
+  <si>
+    <t>chicken</t>
+  </si>
+  <si>
+    <t>dime</t>
+  </si>
+  <si>
+    <t>jam</t>
+  </si>
+  <si>
+    <t>chestnut</t>
+  </si>
+  <si>
+    <t>chipmunk</t>
+  </si>
+  <si>
+    <t>faucet</t>
+  </si>
+  <si>
+    <t>ketchup</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>crow</t>
+  </si>
+  <si>
+    <t>football</t>
+  </si>
+  <si>
+    <t>lemonade</t>
+  </si>
+  <si>
+    <t>cranberry</t>
+  </si>
+  <si>
+    <t>dog</t>
+  </si>
+  <si>
+    <t>glass</t>
+  </si>
+  <si>
+    <t>medicine</t>
+  </si>
+  <si>
+    <t>cucumber</t>
+  </si>
+  <si>
+    <t>dolphin</t>
+  </si>
+  <si>
+    <t>hairbrush</t>
+  </si>
+  <si>
+    <t>mustard</t>
+  </si>
+  <si>
+    <t>dandelion</t>
+  </si>
+  <si>
+    <t>duck</t>
+  </si>
+  <si>
+    <t>hoe</t>
+  </si>
+  <si>
+    <t>pie</t>
+  </si>
+  <si>
+    <t>eggplant</t>
+  </si>
+  <si>
+    <t>elephant</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>rum</t>
+  </si>
+  <si>
+    <t>elm</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>spaghetti</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>goldfish</t>
+  </si>
+  <si>
+    <t>megaphone</t>
+  </si>
+  <si>
+    <t>tea</t>
+  </si>
+  <si>
+    <t>ivy</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>tobacco</t>
+  </si>
+  <si>
+    <t>mushroom</t>
+  </si>
+  <si>
+    <t>hawk</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>oak</t>
+  </si>
+  <si>
+    <t>horse</t>
+  </si>
+  <si>
+    <t>pencil</t>
+  </si>
+  <si>
+    <t>pea</t>
+  </si>
+  <si>
+    <t>monkey</t>
+  </si>
+  <si>
+    <t>rake</t>
+  </si>
+  <si>
+    <t>pineapple</t>
+  </si>
+  <si>
+    <t>moose</t>
+  </si>
+  <si>
+    <t>sandpaper</t>
+  </si>
+  <si>
+    <t>plum</t>
+  </si>
+  <si>
+    <t>mosquito</t>
+  </si>
+  <si>
+    <t>scissors</t>
+  </si>
+  <si>
+    <t>pumpkin</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
+    <t>radish</t>
+  </si>
+  <si>
+    <t>penguin</t>
+  </si>
+  <si>
+    <t>stapler</t>
+  </si>
+  <si>
+    <t>raspberry</t>
+  </si>
+  <si>
+    <t>pig</t>
+  </si>
+  <si>
+    <t>toaster</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>salmon</t>
+  </si>
+  <si>
+    <t>umbrella</t>
+  </si>
+  <si>
+    <t>tangerine</t>
+  </si>
+  <si>
+    <t>snake</t>
+  </si>
+  <si>
+    <t>tomato</t>
+  </si>
+  <si>
+    <t>tiger</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>turtle</t>
+  </si>
+  <si>
+    <t>tulip</t>
+  </si>
+  <si>
+    <t>whale</t>
   </si>
 </sst>
 </file>
@@ -406,11 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +692,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="193" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,386 +720,386 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="2" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="2" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2" t="s">
-        <v>76</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="2" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>108</v>

</xml_diff>